<commit_message>
gets store from user
</commit_message>
<xml_diff>
--- a/quick_eval_store_data.xlsx
+++ b/quick_eval_store_data.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="200">
   <si>
     <t xml:space="preserve">the body shop </t>
   </si>
@@ -615,13 +616,22 @@
   </si>
   <si>
     <t>water world</t>
+  </si>
+  <si>
+    <t>huhot</t>
+  </si>
+  <si>
+    <t>50x8</t>
+  </si>
+  <si>
+    <t>jimmy johns</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1069,11 +1079,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36:X36"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
@@ -1089,7 +1099,7 @@
     <col min="25" max="25" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -1147,7 +1157,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="16.2" customHeight="1">
+    <row r="2" spans="1:26" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1213,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="30">
+    <row r="3" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1262,7 +1272,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="22.2" customHeight="1">
+    <row r="5" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1362,7 +1372,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1402,7 +1412,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="30">
+    <row r="7" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1456,7 +1466,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30">
+    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1518,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="30">
+    <row r="9" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1557,7 +1567,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="30">
+    <row r="10" spans="1:26" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1610,7 +1620,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15">
+    <row r="11" spans="1:26" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="G12" s="14">
         <v>1</v>
       </c>
@@ -1711,7 +1721,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1762,7 +1772,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1806,7 +1816,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -1850,7 +1860,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15">
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1942,7 +1952,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>63</v>
       </c>
@@ -1991,7 +2001,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -2026,7 +2036,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -2122,7 +2132,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2166,7 +2176,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2213,7 +2223,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2245,7 +2255,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -2291,7 +2301,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2304,6 +2314,19 @@
       <c r="G26" s="14">
         <v>1</v>
       </c>
+      <c r="H26" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>156</v>
+      </c>
       <c r="T26" t="s">
         <v>179</v>
       </c>
@@ -2320,7 +2343,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -2346,7 +2369,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -2372,7 +2395,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -2398,7 +2421,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -2424,7 +2447,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -2450,7 +2473,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2476,7 +2499,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -2502,7 +2525,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -2528,7 +2551,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2554,7 +2577,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -2583,7 +2606,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -2609,7 +2632,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -2635,7 +2658,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>128</v>
       </c>
@@ -2661,7 +2684,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>129</v>
       </c>
@@ -2687,7 +2710,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>130</v>
       </c>
@@ -2697,8 +2720,22 @@
       <c r="D41">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:25">
+      <c r="T41" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="U41" s="22"/>
+      <c r="V41" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="W41" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="X41" s="22"/>
+      <c r="Y41" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>134</v>
       </c>
@@ -2709,7 +2746,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -2765,8 +2802,11 @@
     <hyperlink ref="Y7" r:id="rId41"/>
     <hyperlink ref="Y8" r:id="rId42"/>
     <hyperlink ref="W27:W40" r:id="rId43" display="https://shoppy.gg/@wild"/>
+    <hyperlink ref="L26" r:id="rId44"/>
+    <hyperlink ref="Y41" r:id="rId45"/>
+    <hyperlink ref="W41" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>